<commit_message>
Latest Member List Update & Pic OCR Processed
</commit_message>
<xml_diff>
--- a/4.11-4.17.xlsx
+++ b/4.11-4.17.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="掠夺总榜" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="157">
   <si>
     <t>ID</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>KILL</t>
   </si>
   <si>
@@ -422,6 +419,90 @@
   </si>
   <si>
     <t>古手梨花sama</t>
+  </si>
+  <si>
+    <t>凰荼歌</t>
+  </si>
+  <si>
+    <t>古巷烟雨断桥殇</t>
+  </si>
+  <si>
+    <t>时钟轻摇孤独</t>
+  </si>
+  <si>
+    <t>亲爱的未闻花名</t>
+  </si>
+  <si>
+    <t>柒叶浅</t>
+  </si>
+  <si>
+    <t>梦觞丶</t>
+  </si>
+  <si>
+    <t>老滚</t>
+  </si>
+  <si>
+    <t>万心忧</t>
+  </si>
+  <si>
+    <t>君挽言</t>
+  </si>
+  <si>
+    <t>我是恺子爸</t>
+  </si>
+  <si>
+    <t>意邪</t>
+  </si>
+  <si>
+    <t>放肆流逝的年华</t>
+  </si>
+  <si>
+    <t>池小晚</t>
+  </si>
+  <si>
+    <t>清弦</t>
+  </si>
+  <si>
+    <t>全城竟是小白兔</t>
+  </si>
+  <si>
+    <t>蚩尤魔人</t>
+  </si>
+  <si>
+    <t>阿锟猫</t>
+  </si>
+  <si>
+    <t>最可爱的师姐</t>
+  </si>
+  <si>
+    <t>彡电竞丿柯南乄</t>
+  </si>
+  <si>
+    <t>浩浩丶浩</t>
+  </si>
+  <si>
+    <t>若火流星 煌煌</t>
+  </si>
+  <si>
+    <t>董汉卿</t>
+  </si>
+  <si>
+    <t>那年红颜</t>
+  </si>
+  <si>
+    <t>＊下水道的白</t>
+  </si>
+  <si>
+    <t>一人一枪闯九州</t>
+  </si>
+  <si>
+    <t>叁岁丶</t>
+  </si>
+  <si>
+    <t>晓月梦澈</t>
+  </si>
+  <si>
+    <t>树儿高高长</t>
   </si>
 </sst>
 </file>
@@ -486,14 +567,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -777,44 +858,45 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S91"/>
+  <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="Q1" s="4" t="s">
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="Q1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -864,14 +946,17 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -879,7 +964,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -887,7 +978,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -895,7 +992,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -903,7 +1006,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -911,7 +1020,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -919,7 +1034,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -927,7 +1048,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="E10" s="3">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -935,7 +1062,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="E11" s="3">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -943,7 +1076,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="E12" s="3">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -951,7 +1090,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="E13" s="3">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -959,7 +1104,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E14" s="3">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -967,7 +1118,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="E15" s="3">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -975,607 +1132,1119 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E16" s="3">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E18" s="3">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="E19" s="3">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E20" s="3">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="E21" s="3">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E22" s="3">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E23" s="3">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E24" s="3">
+        <v>22</v>
+      </c>
+      <c r="F24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E25" s="3">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E26" s="3">
+        <v>24</v>
+      </c>
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E27" s="3">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E28" s="3">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E29" s="3">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E30" s="3">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E31" s="3">
+        <v>29</v>
+      </c>
+      <c r="F31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E32" s="3">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E33" s="3">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E34" s="3">
+        <v>32</v>
+      </c>
+      <c r="F34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="E35" s="3">
+        <v>33</v>
+      </c>
+      <c r="F35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="E36" s="3">
+        <v>34</v>
+      </c>
+      <c r="F36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="E37" s="3">
+        <v>35</v>
+      </c>
+      <c r="F37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="E38" s="3">
+        <v>36</v>
+      </c>
+      <c r="F38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E39" s="3">
+        <v>37</v>
+      </c>
+      <c r="F39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="E40" s="3">
+        <v>38</v>
+      </c>
+      <c r="F40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E41" s="3">
+        <v>39</v>
+      </c>
+      <c r="F41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="E42" s="3">
+        <v>40</v>
+      </c>
+      <c r="F42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E43" s="3">
+        <v>41</v>
+      </c>
+      <c r="F43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E44" s="3">
+        <v>42</v>
+      </c>
+      <c r="F44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E45" s="3">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E46" s="3">
+        <v>44</v>
+      </c>
+      <c r="F46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E47" s="3">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E48" s="3">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E49" s="3">
+        <v>47</v>
+      </c>
+      <c r="F49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E50" s="3">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E51" s="3">
+        <v>49</v>
+      </c>
+      <c r="F51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E52" s="3">
+        <v>50</v>
+      </c>
+      <c r="F52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E53" s="3">
+        <v>51</v>
+      </c>
+      <c r="F53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="E54" s="3">
+        <v>52</v>
+      </c>
+      <c r="F54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E55" s="3">
+        <v>53</v>
+      </c>
+      <c r="F55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E56" s="3">
+        <v>54</v>
+      </c>
+      <c r="F56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="E57" s="3">
+        <v>55</v>
+      </c>
+      <c r="F57" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="E58" s="3">
+        <v>56</v>
+      </c>
+      <c r="F58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="E59" s="3">
+        <v>57</v>
+      </c>
+      <c r="F59" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="E60" s="3">
+        <v>58</v>
+      </c>
+      <c r="F60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="E61" s="3">
+        <v>59</v>
+      </c>
+      <c r="F61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="E62" s="3">
+        <v>60</v>
+      </c>
+      <c r="F62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="E63" s="3">
+        <v>61</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="E64" s="3">
+        <v>62</v>
+      </c>
+      <c r="F64" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="E65" s="3">
+        <v>63</v>
+      </c>
+      <c r="F65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="E66" s="3">
+        <v>64</v>
+      </c>
+      <c r="F66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="E67" s="3">
+        <v>65</v>
+      </c>
+      <c r="F67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E68" s="3">
+        <v>66</v>
+      </c>
+      <c r="F68" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="E69" s="3">
+        <v>67</v>
+      </c>
+      <c r="F69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E70" s="3">
+        <v>68</v>
+      </c>
+      <c r="F70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="E71" s="3">
+        <v>69</v>
+      </c>
+      <c r="F71" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="E72" s="3">
+        <v>70</v>
+      </c>
+      <c r="F72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>71</v>
       </c>
       <c r="B73" t="s">
+        <v>93</v>
+      </c>
+      <c r="E73" s="3">
+        <v>71</v>
+      </c>
+      <c r="F73" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="E74" s="3">
+        <v>72</v>
+      </c>
+      <c r="F74" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="E75" s="3">
+        <v>73</v>
+      </c>
+      <c r="F75" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="E76" s="3">
+        <v>74</v>
+      </c>
+      <c r="F76" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="E77" s="3">
+        <v>75</v>
+      </c>
+      <c r="F77" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E78" s="3">
+        <v>76</v>
+      </c>
+      <c r="F78" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E79" s="3">
+        <v>77</v>
+      </c>
+      <c r="F79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="E80" s="3">
+        <v>78</v>
+      </c>
+      <c r="F80" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="E81" s="3">
+        <v>79</v>
+      </c>
+      <c r="F81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="E82" s="3">
+        <v>80</v>
+      </c>
+      <c r="F82" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E83" s="3">
+        <v>81</v>
+      </c>
+      <c r="F83" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="E84" s="3">
+        <v>82</v>
+      </c>
+      <c r="F84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E85" s="3">
+        <v>83</v>
+      </c>
+      <c r="F85" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="E86" s="3">
+        <v>84</v>
+      </c>
+      <c r="F86" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="E87" s="3">
+        <v>85</v>
+      </c>
+      <c r="F87" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="E88" s="3">
+        <v>86</v>
+      </c>
+      <c r="F88" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="E89" s="3">
+        <v>87</v>
+      </c>
+      <c r="F89" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="E90" s="3">
+        <v>88</v>
+      </c>
+      <c r="F90" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="E91" s="3">
+        <v>89</v>
+      </c>
+      <c r="F91" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="E92" s="4">
+        <v>90</v>
+      </c>
+      <c r="F92" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E93" s="3">
+        <v>91</v>
+      </c>
+      <c r="F93" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E94" s="3">
+        <v>92</v>
+      </c>
+      <c r="F94" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E95" s="3">
+        <v>93</v>
+      </c>
+      <c r="F95" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E96" s="3">
+        <v>94</v>
+      </c>
+      <c r="F96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E97" s="3">
+        <v>95</v>
+      </c>
+      <c r="F97" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="98" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E98" s="3">
+        <v>96</v>
+      </c>
+      <c r="F98" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1603,14 +2272,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1645,97 +2314,97 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="A2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1744,7 +2413,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1753,7 +2422,7 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1762,7 +2431,7 @@
         <v>9</v>
       </c>
       <c r="M4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1773,7 +2442,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1782,7 +2451,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1791,7 +2460,7 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1800,7 +2469,7 @@
         <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1811,7 +2480,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1820,7 +2489,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1829,7 +2498,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1838,7 +2507,7 @@
         <v>6</v>
       </c>
       <c r="M6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1849,7 +2518,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1858,7 +2527,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -1867,7 +2536,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1876,7 +2545,7 @@
         <v>11</v>
       </c>
       <c r="M7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1887,7 +2556,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1896,7 +2565,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1905,7 +2574,7 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J8">
         <v>7</v>
@@ -1914,7 +2583,7 @@
         <v>41</v>
       </c>
       <c r="M8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1925,7 +2594,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1934,7 +2603,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1943,7 +2612,7 @@
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1952,7 +2621,7 @@
         <v>4</v>
       </c>
       <c r="M9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1963,7 +2632,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1972,7 +2641,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1981,7 +2650,7 @@
         <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1990,7 +2659,7 @@
         <v>7</v>
       </c>
       <c r="M10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N10">
         <v>4</v>
@@ -2001,7 +2670,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2010,7 +2679,7 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -2019,7 +2688,7 @@
         <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2028,7 +2697,7 @@
         <v>13</v>
       </c>
       <c r="M11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2039,7 +2708,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2048,7 +2717,7 @@
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12">
         <v>12</v>
@@ -2057,7 +2726,7 @@
         <v>35</v>
       </c>
       <c r="M12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -2068,7 +2737,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2077,7 +2746,7 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J13">
         <v>16</v>
@@ -2086,7 +2755,7 @@
         <v>29</v>
       </c>
       <c r="M13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -2097,7 +2766,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -2106,7 +2775,7 @@
         <v>7</v>
       </c>
       <c r="M14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2117,7 +2786,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -2126,7 +2795,7 @@
         <v>4</v>
       </c>
       <c r="M15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -2184,7 +2853,7 @@
       </c>
       <c r="B2" s="2">
         <f>COUNTIF(掠夺总榜!A$1:S$140,$A2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>COUNTIF(盟会战!A$1:S$140,$A2)</f>
@@ -2196,7 +2865,7 @@
       </c>
       <c r="E2">
         <f>SUM(B2,C2,D2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2016-04-15帮战(龙狗) DATA & MACRO EDIT
</commit_message>
<xml_diff>
--- a/4.11-4.17.xlsx
+++ b/4.11-4.17.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="掠夺总榜" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="197">
   <si>
     <t>ID</t>
   </si>
@@ -617,6 +617,12 @@
   </si>
   <si>
     <t>风暖伤</t>
+  </si>
+  <si>
+    <t>2016-04-15-龙狗</t>
+  </si>
+  <si>
+    <t>总计</t>
   </si>
 </sst>
 </file>
@@ -672,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -690,6 +696,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="好" xfId="1" builtinId="26"/>
@@ -706,6 +715,2699 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>帮战总榜!$Q$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KILL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>帮战总榜!$R$17:$U$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>逐梦</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>如梦</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>若梦</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>何梦</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>帮战总榜!$R$18:$U$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-01F4-400D-AE4A-8DE0F1DB7D66}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>帮战总榜!$Q$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ASS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>帮战总榜!$R$17:$U$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>逐梦</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>如梦</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>若梦</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>何梦</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>帮战总榜!$R$19:$U$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>184</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-01F4-400D-AE4A-8DE0F1DB7D66}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="408576224"/>
+        <c:axId val="408573312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="408576224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="408573312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="408573312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="408576224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>助攻</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.45143044619422573"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>帮战总榜!$Q$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ASS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>帮战总榜!$R$17:$U$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>逐梦</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>如梦</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>若梦</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>何梦</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>帮战总榜!$R$19:$U$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>184</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-62A3-4EEC-8BEB-0286FE695269}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>击杀</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>帮战总榜!$Q$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KILL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>帮战总榜!$R$17:$U$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>逐梦</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>如梦</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>若梦</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>何梦</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>帮战总榜!$R$18:$U$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3BF6-4486-8673-C42428A57BD5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -974,8 +3676,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q1:Q1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4334,13 +7036,19 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="AE28" sqref="AE28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
@@ -4826,8 +7534,1089 @@
         <v>5</v>
       </c>
     </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="R17" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" t="s">
+        <v>4</v>
+      </c>
+      <c r="T17" t="s">
+        <v>5</v>
+      </c>
+      <c r="U17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18">
+        <v>22</v>
+      </c>
+      <c r="S18">
+        <v>11</v>
+      </c>
+      <c r="T18">
+        <v>39</v>
+      </c>
+      <c r="U18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7">
+        <v>25</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
+        <v>7</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7">
+        <v>10</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="N19" s="7">
+        <v>0</v>
+      </c>
+      <c r="O19" s="7">
+        <v>17</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19">
+        <v>254</v>
+      </c>
+      <c r="S19">
+        <v>255</v>
+      </c>
+      <c r="T19">
+        <v>554</v>
+      </c>
+      <c r="U19">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7">
+        <v>14</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7">
+        <v>21</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="7">
+        <v>3</v>
+      </c>
+      <c r="K20" s="7">
+        <v>21</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0</v>
+      </c>
+      <c r="O20" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="7">
+        <v>2</v>
+      </c>
+      <c r="C21" s="7">
+        <v>9</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7">
+        <v>12</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J21" s="7">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7">
+        <v>23</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N21" s="7">
+        <v>1</v>
+      </c>
+      <c r="O21" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0</v>
+      </c>
+      <c r="C22" s="7">
+        <v>18</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <v>27</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="7">
+        <v>2</v>
+      </c>
+      <c r="K22" s="7">
+        <v>49</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="N22" s="7">
+        <v>3</v>
+      </c>
+      <c r="O22" s="7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2</v>
+      </c>
+      <c r="C23" s="7">
+        <v>20</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7">
+        <v>24</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J23" s="7">
+        <v>0</v>
+      </c>
+      <c r="K23" s="7">
+        <v>8</v>
+      </c>
+      <c r="L23" s="7"/>
+      <c r="M23" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N23" s="7">
+        <v>0</v>
+      </c>
+      <c r="O23" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" s="7">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7">
+        <v>20</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>15</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J24" s="7">
+        <v>4</v>
+      </c>
+      <c r="K24" s="7">
+        <v>22</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="N24" s="7">
+        <v>0</v>
+      </c>
+      <c r="O24" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="7">
+        <v>5</v>
+      </c>
+      <c r="C25" s="7">
+        <v>15</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7">
+        <v>34</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J25" s="7">
+        <v>2</v>
+      </c>
+      <c r="K25" s="7">
+        <v>4</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N25" s="7">
+        <v>1</v>
+      </c>
+      <c r="O25" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7">
+        <v>15</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
+      <c r="G26" s="7">
+        <v>38</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7">
+        <v>4</v>
+      </c>
+      <c r="L26" s="7"/>
+      <c r="M26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="N26" s="7">
+        <v>1</v>
+      </c>
+      <c r="O26" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7">
+        <v>6</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7">
+        <v>3</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="7">
+        <v>3</v>
+      </c>
+      <c r="K27" s="7">
+        <v>23</v>
+      </c>
+      <c r="L27" s="7"/>
+      <c r="M27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N27" s="7">
+        <v>1</v>
+      </c>
+      <c r="O27" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="7">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7">
+        <v>23</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+      <c r="G28" s="7">
+        <v>4</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
+        <v>21</v>
+      </c>
+      <c r="L28" s="7"/>
+      <c r="M28" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N28" s="7">
+        <v>0</v>
+      </c>
+      <c r="O28" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>12</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7">
+        <v>14</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7">
+        <v>14</v>
+      </c>
+      <c r="L29" s="7"/>
+      <c r="M29" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N29" s="7">
+        <v>0</v>
+      </c>
+      <c r="O29" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0</v>
+      </c>
+      <c r="C30" s="7">
+        <v>4</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7">
+        <v>9</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J30" s="7">
+        <v>2</v>
+      </c>
+      <c r="K30" s="7">
+        <v>33</v>
+      </c>
+      <c r="L30" s="7"/>
+      <c r="M30" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N30" s="7">
+        <v>2</v>
+      </c>
+      <c r="O30" s="7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7">
+        <v>2</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0</v>
+      </c>
+      <c r="G31" s="7">
+        <v>6</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="7">
+        <v>1</v>
+      </c>
+      <c r="K31" s="7">
+        <v>3</v>
+      </c>
+      <c r="L31" s="7"/>
+      <c r="M31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N31" s="7">
+        <v>0</v>
+      </c>
+      <c r="O31" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0</v>
+      </c>
+      <c r="C32" s="7">
+        <v>5</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0</v>
+      </c>
+      <c r="G32" s="7">
+        <v>3</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J32" s="7">
+        <v>1</v>
+      </c>
+      <c r="K32" s="7">
+        <v>6</v>
+      </c>
+      <c r="L32" s="7"/>
+      <c r="M32" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N32" s="7">
+        <v>0</v>
+      </c>
+      <c r="O32" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="7">
+        <v>0</v>
+      </c>
+      <c r="C33" s="7">
+        <v>26</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7">
+        <v>27</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33" s="7">
+        <v>2</v>
+      </c>
+      <c r="K33" s="7">
+        <v>24</v>
+      </c>
+      <c r="L33" s="7"/>
+      <c r="M33" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="N33" s="7">
+        <v>2</v>
+      </c>
+      <c r="O33" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="7">
+        <v>3</v>
+      </c>
+      <c r="C34" s="7">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7">
+        <v>11</v>
+      </c>
+      <c r="H34" s="7"/>
+      <c r="I34" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="J34" s="7">
+        <v>1</v>
+      </c>
+      <c r="K34" s="7">
+        <v>6</v>
+      </c>
+      <c r="L34" s="7"/>
+      <c r="M34" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="N34" s="7">
+        <f>SUM(N19:N33)</f>
+        <v>11</v>
+      </c>
+      <c r="O34" s="7">
+        <f>SUM(O19:O33)</f>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7">
+        <v>16</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F35" s="7">
+        <f>SUM(F19:F34)</f>
+        <v>11</v>
+      </c>
+      <c r="G35" s="7">
+        <f>SUM(G19:G34)</f>
+        <v>255</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J35" s="7">
+        <v>1</v>
+      </c>
+      <c r="K35" s="7">
+        <v>2</v>
+      </c>
+      <c r="L35" s="7"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B36" s="7">
+        <f>SUM(B19:B35)</f>
+        <v>22</v>
+      </c>
+      <c r="C36" s="7">
+        <f>SUM(C19:C35)</f>
+        <v>254</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J36" s="7">
+        <v>4</v>
+      </c>
+      <c r="K36" s="7">
+        <v>47</v>
+      </c>
+      <c r="L36" s="7"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J37" s="7">
+        <v>0</v>
+      </c>
+      <c r="K37" s="7">
+        <v>30</v>
+      </c>
+      <c r="L37" s="7"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="Y37" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="5"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J38" s="7">
+        <v>4</v>
+      </c>
+      <c r="K38" s="7">
+        <v>21</v>
+      </c>
+      <c r="L38" s="7"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="J39" s="7">
+        <v>1</v>
+      </c>
+      <c r="K39" s="7">
+        <v>28</v>
+      </c>
+      <c r="L39" s="7"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J40" s="7">
+        <v>1</v>
+      </c>
+      <c r="K40" s="7">
+        <v>17</v>
+      </c>
+      <c r="L40" s="7"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J41" s="7">
+        <v>0</v>
+      </c>
+      <c r="K41" s="7">
+        <v>14</v>
+      </c>
+      <c r="L41" s="7"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="7">
+        <v>0</v>
+      </c>
+      <c r="K42" s="7">
+        <v>8</v>
+      </c>
+      <c r="L42" s="7"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J43" s="7">
+        <v>5</v>
+      </c>
+      <c r="K43" s="7">
+        <v>36</v>
+      </c>
+      <c r="L43" s="7"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J44" s="7">
+        <v>1</v>
+      </c>
+      <c r="K44" s="7">
+        <v>27</v>
+      </c>
+      <c r="L44" s="7"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J45" s="7">
+        <v>0</v>
+      </c>
+      <c r="K45" s="7">
+        <v>6</v>
+      </c>
+      <c r="L45" s="7"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J46" s="7">
+        <v>1</v>
+      </c>
+      <c r="K46" s="7">
+        <v>40</v>
+      </c>
+      <c r="L46" s="7"/>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J47" s="7">
+        <v>0</v>
+      </c>
+      <c r="K47" s="7">
+        <v>7</v>
+      </c>
+      <c r="L47" s="7"/>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J48" s="7">
+        <f>SUM(J19:J47)</f>
+        <v>39</v>
+      </c>
+      <c r="K48" s="7">
+        <f>SUM(K19:K47)</f>
+        <v>554</v>
+      </c>
+      <c r="L48" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="Y37:AB37"/>
+    <mergeCell ref="A17:O17"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
@@ -4835,6 +8624,7 @@
     <mergeCell ref="A2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5009,7 +8799,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>